<commit_message>
Lab 3 - Final version, to revise
</commit_message>
<xml_diff>
--- a/Lab3/pipeline_1_byhand.xlsx
+++ b/Lab3/pipeline_1_byhand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\michele\uni\polito\quarto_anno\primo_semestre\architetture_sistemi_elaborazione\laboratori\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B86FFA-8BA6-45B9-866E-A20D4C4CAE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B8B6FA-808E-41F8-9F4A-86FC889C5CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7596" yWindow="204" windowWidth="15300" windowHeight="11436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Even" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="62">
   <si>
     <t>daddui R1, R0, 0</t>
   </si>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4226C58-3B8B-4FE1-9213-2384D9B32338}">
   <dimension ref="A1:EG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG9" zoomScale="102" workbookViewId="0">
-      <selection activeCell="CP44" sqref="CP44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="102" workbookViewId="0">
+      <selection activeCell="CQ43" sqref="CQ43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3647,18 +3647,15 @@
         <v>20</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF20" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AI20" s="1"/>
@@ -3719,7 +3716,7 @@
       <c r="CM20" s="3"/>
       <c r="CN20" s="3"/>
       <c r="CO20" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CP20" s="3"/>
       <c r="CQ20" s="3"/>
@@ -3798,22 +3795,22 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
+      <c r="AD21" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AE21" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF21" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG21" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI21" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
@@ -3840,7 +3837,7 @@
       <c r="BG21" s="1"/>
       <c r="BH21" s="1"/>
       <c r="BI21" s="1"/>
-      <c r="BJ21" s="1"/>
+      <c r="BJ21" s="3"/>
       <c r="BK21" s="3"/>
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
@@ -3862,7 +3859,6 @@
       <c r="CC21" s="3"/>
       <c r="CD21" s="3"/>
       <c r="CE21" s="3"/>
-      <c r="CF21" s="3"/>
       <c r="CH21" s="3"/>
       <c r="CI21" s="3"/>
       <c r="CJ21" s="3"/>
@@ -3951,9 +3947,11 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
-      <c r="AE22" s="1"/>
+      <c r="AE22" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AF22" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="AG22" s="1" t="s">
         <v>55</v>
@@ -3964,9 +3962,7 @@
       <c r="AI22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AJ22" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
@@ -3992,7 +3988,7 @@
       <c r="BG22" s="1"/>
       <c r="BH22" s="1"/>
       <c r="BI22" s="1"/>
-      <c r="BJ22" s="1"/>
+      <c r="BJ22" s="3"/>
       <c r="BK22" s="3"/>
       <c r="BL22" s="3"/>
       <c r="BM22" s="3"/>
@@ -4014,7 +4010,6 @@
       <c r="CC22" s="3"/>
       <c r="CD22" s="3"/>
       <c r="CE22" s="3"/>
-      <c r="CF22" s="3"/>
       <c r="CH22" s="3"/>
       <c r="CI22" s="3"/>
       <c r="CJ22" s="3"/>
@@ -4104,12 +4099,14 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
       <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
+      <c r="AF23" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AG23" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="AI23" s="1" t="s">
         <v>24</v>
@@ -4151,7 +4148,7 @@
       <c r="BB23" s="1"/>
       <c r="BC23" s="1"/>
       <c r="BD23" s="1"/>
-      <c r="BE23" s="1"/>
+      <c r="BE23" s="3"/>
       <c r="BF23" s="3"/>
       <c r="BG23" s="3"/>
       <c r="BH23" s="3"/>
@@ -4178,12 +4175,11 @@
       <c r="CC23" s="3"/>
       <c r="CD23" s="3"/>
       <c r="CE23" s="3"/>
-      <c r="CF23" s="3"/>
       <c r="CH23" s="3"/>
       <c r="CI23" s="3"/>
       <c r="CJ23" s="3"/>
       <c r="CO23" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="CP23" s="3"/>
       <c r="CQ23" s="3"/>
@@ -4264,13 +4260,15 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
-      <c r="AF24" s="3"/>
-      <c r="AG24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AH24" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="AJ24" s="1" t="s">
         <v>20</v>
@@ -4287,7 +4285,7 @@
       <c r="AN24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AO24" s="1" t="s">
+      <c r="AO24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AP24" s="1" t="s">
@@ -4315,7 +4313,7 @@
       <c r="BB24" s="1"/>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1"/>
-      <c r="BE24" s="1"/>
+      <c r="BE24" s="3"/>
       <c r="BF24" s="3"/>
       <c r="BG24" s="3"/>
       <c r="BH24" s="3"/>
@@ -4342,7 +4340,6 @@
       <c r="CC24" s="3"/>
       <c r="CD24" s="3"/>
       <c r="CE24" s="3"/>
-      <c r="CF24" s="3"/>
       <c r="CH24" s="3"/>
       <c r="CI24" s="3"/>
       <c r="CJ24" s="3"/>
@@ -4428,11 +4425,13 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
-      <c r="AF25" s="3"/>
+      <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
+      <c r="AH25" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AI25" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="AJ25" s="1" t="s">
         <v>20</v>
@@ -4458,7 +4457,7 @@
       <c r="AQ25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AR25" s="1" t="s">
+      <c r="AR25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AS25" s="1" t="s">
@@ -4483,7 +4482,7 @@
       <c r="BB25" s="1"/>
       <c r="BC25" s="1"/>
       <c r="BD25" s="1"/>
-      <c r="BE25" s="1"/>
+      <c r="BE25" s="3"/>
       <c r="BF25" s="3"/>
       <c r="BG25" s="3"/>
       <c r="BH25" s="3"/>
@@ -4510,7 +4509,6 @@
       <c r="CC25" s="3"/>
       <c r="CD25" s="3"/>
       <c r="CE25" s="3"/>
-      <c r="CF25" s="3"/>
       <c r="CH25" s="3"/>
       <c r="CI25" s="3"/>
       <c r="CJ25" s="3"/>
@@ -4596,7 +4594,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
+      <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
@@ -4605,7 +4603,6 @@
       <c r="AL26" s="1"/>
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
-      <c r="AO26" s="1"/>
       <c r="AP26" s="1" t="s">
         <v>1</v>
       </c>
@@ -4639,7 +4636,7 @@
       <c r="BB26" s="1"/>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1"/>
-      <c r="BE26" s="1"/>
+      <c r="BE26" s="3"/>
       <c r="BF26" s="3"/>
       <c r="BG26" s="3"/>
       <c r="BH26" s="3"/>
@@ -4666,7 +4663,6 @@
       <c r="CC26" s="3"/>
       <c r="CD26" s="3"/>
       <c r="CE26" s="3"/>
-      <c r="CF26" s="3"/>
       <c r="CH26" s="3"/>
       <c r="CI26" s="3"/>
       <c r="CJ26" s="3"/>
@@ -4752,7 +4748,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
-      <c r="AF27" s="3"/>
+      <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
@@ -4764,38 +4760,35 @@
       <c r="AO27" s="1"/>
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
-      <c r="AR27" s="1"/>
+      <c r="AR27" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AS27" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT27" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="AU27" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="AV27" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="AW27" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="AX27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AY27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AZ27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BA27" s="1" t="s">
+      <c r="AY27" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="BA27" s="1"/>
       <c r="BB27" s="1"/>
       <c r="BC27" s="1"/>
       <c r="BD27" s="1"/>
-      <c r="BE27" s="1"/>
+      <c r="BE27" s="3"/>
       <c r="BF27" s="3"/>
       <c r="BG27" s="3"/>
       <c r="BH27" s="3"/>
@@ -4822,12 +4815,11 @@
       <c r="CC27" s="3"/>
       <c r="CD27" s="3"/>
       <c r="CE27" s="3"/>
-      <c r="CF27" s="3"/>
       <c r="CH27" s="3"/>
       <c r="CI27" s="3"/>
       <c r="CJ27" s="3"/>
       <c r="CO27" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="CP27" s="3"/>
       <c r="CQ27" s="3"/>
@@ -4908,7 +4900,7 @@
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
       <c r="AE28" s="3"/>
-      <c r="AF28" s="3"/>
+      <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
@@ -4921,24 +4913,26 @@
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
       <c r="AR28" s="1"/>
-      <c r="AS28" s="1"/>
+      <c r="AS28" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AT28" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="AU28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="AV28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AW28" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AW28" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="AX28" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="AY28" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="AZ28" s="1" t="s">
         <v>53</v>
@@ -4994,18 +4988,13 @@
       <c r="BQ28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BR28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BS28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BT28" s="3" t="s">
+      <c r="BR28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="BU28" s="3" t="s">
+      <c r="BS28" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="BU28" s="3"/>
       <c r="BV28" s="3"/>
       <c r="BW28" s="3"/>
       <c r="BX28" s="3"/>
@@ -5016,7 +5005,6 @@
       <c r="CC28" s="3"/>
       <c r="CD28" s="3"/>
       <c r="CE28" s="3"/>
-      <c r="CF28" s="3"/>
       <c r="CH28" s="3"/>
       <c r="CI28" s="3"/>
       <c r="CJ28" s="3"/>
@@ -5102,7 +5090,7 @@
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
-      <c r="AF29" s="3"/>
+      <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
@@ -5118,21 +5106,23 @@
       <c r="AS29" s="1"/>
       <c r="AT29" s="1"/>
       <c r="AU29" s="1"/>
-      <c r="AV29" s="1"/>
+      <c r="AV29" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AW29" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="AX29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="AY29" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="AZ29" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA29" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="BB29" s="1" t="s">
         <v>20</v>
@@ -5143,7 +5133,7 @@
       <c r="BD29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="BE29" s="1" t="s">
+      <c r="BE29" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BF29" s="3" t="s">
@@ -5186,17 +5176,12 @@
         <v>20</v>
       </c>
       <c r="BS29" s="3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="BT29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="BU29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="BV29" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="BV29" s="3"/>
       <c r="BW29" s="3"/>
       <c r="BX29" s="3"/>
       <c r="BY29" s="3"/>
@@ -5206,7 +5191,6 @@
       <c r="CC29" s="3"/>
       <c r="CD29" s="3"/>
       <c r="CE29" s="3"/>
-      <c r="CF29" s="3"/>
       <c r="CH29" s="3"/>
       <c r="CI29" s="3"/>
       <c r="CJ29" s="3"/>
@@ -5292,7 +5276,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
-      <c r="AF30" s="3"/>
+      <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
@@ -5311,12 +5295,14 @@
       <c r="AV30" s="1"/>
       <c r="AW30" s="1"/>
       <c r="AX30" s="1"/>
-      <c r="AY30" s="1"/>
+      <c r="AY30" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AZ30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA30" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="BB30" s="1" t="s">
         <v>54</v>
@@ -5325,14 +5311,12 @@
         <v>54</v>
       </c>
       <c r="BD30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BE30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BF30" s="3" t="s">
+      <c r="BE30" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="BF30" s="3"/>
       <c r="BG30" s="3"/>
       <c r="BH30" s="3"/>
       <c r="BI30" s="3"/>
@@ -5358,7 +5342,6 @@
       <c r="CC30" s="3"/>
       <c r="CD30" s="3"/>
       <c r="CE30" s="3"/>
-      <c r="CF30" s="3"/>
       <c r="CH30" s="3"/>
       <c r="CI30" s="3"/>
       <c r="CJ30" s="3"/>
@@ -5444,7 +5427,7 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3"/>
-      <c r="AF31" s="3"/>
+      <c r="AF31" s="1"/>
       <c r="AG31" s="1"/>
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
@@ -5464,12 +5447,14 @@
       <c r="AW31" s="1"/>
       <c r="AX31" s="1"/>
       <c r="AY31" s="1"/>
-      <c r="AZ31" s="1"/>
+      <c r="AZ31" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="BA31" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB31" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="BC31" s="1" t="s">
         <v>20</v>
@@ -5477,7 +5462,7 @@
       <c r="BD31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="BE31" s="1" t="s">
+      <c r="BE31" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BF31" s="3" t="s">
@@ -5517,10 +5502,10 @@
         <v>20</v>
       </c>
       <c r="BR31" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="BS31" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="BT31" s="3" t="s">
         <v>24</v>
@@ -5541,20 +5526,14 @@
         <v>24</v>
       </c>
       <c r="BZ31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="CA31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="CB31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="CC31" s="4" t="s">
+      <c r="CA31" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="CC31" s="3"/>
       <c r="CD31" s="3"/>
       <c r="CE31" s="3"/>
-      <c r="CF31" s="3"/>
       <c r="CH31" s="3"/>
       <c r="CI31" s="3"/>
       <c r="CJ31" s="3"/>
@@ -5640,7 +5619,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
-      <c r="AF32" s="3"/>
+      <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
@@ -5661,9 +5640,11 @@
       <c r="AX32" s="1"/>
       <c r="AY32" s="1"/>
       <c r="AZ32" s="1"/>
-      <c r="BA32" s="1"/>
+      <c r="BA32" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="BB32" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="BC32" s="1" t="s">
         <v>20</v>
@@ -5671,7 +5652,7 @@
       <c r="BD32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="BE32" s="1" t="s">
+      <c r="BE32" s="3" t="s">
         <v>20</v>
       </c>
       <c r="BF32" s="3" t="s">
@@ -5711,16 +5692,16 @@
         <v>20</v>
       </c>
       <c r="BR32" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="BS32" s="3" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="BT32" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="BU32" s="3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="BV32" s="3" t="s">
         <v>20</v>
@@ -5738,19 +5719,13 @@
         <v>20</v>
       </c>
       <c r="CA32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="CB32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="CC32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="CD32" s="4" t="s">
+      <c r="CB32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="CE32" s="3"/>
-      <c r="CF32" s="3"/>
+      <c r="CC32" s="3"/>
+      <c r="CD32" s="3"/>
       <c r="CH32" s="3"/>
       <c r="CI32" s="3"/>
       <c r="CJ32" s="3"/>
@@ -5836,7 +5811,7 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
-      <c r="AF33" s="3"/>
+      <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
@@ -5861,7 +5836,7 @@
       <c r="BB33" s="1"/>
       <c r="BC33" s="1"/>
       <c r="BD33" s="1"/>
-      <c r="BE33" s="1"/>
+      <c r="BE33" s="3"/>
       <c r="BF33" s="3"/>
       <c r="BG33" s="3"/>
       <c r="BH33" s="3"/>
@@ -5874,13 +5849,17 @@
       <c r="BO33" s="3"/>
       <c r="BP33" s="3"/>
       <c r="BQ33" s="3"/>
-      <c r="BR33" s="3"/>
-      <c r="BS33" s="3"/>
+      <c r="BR33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS33" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="BT33" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="BU33" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="BV33" s="3" t="s">
         <v>20</v>
@@ -5894,26 +5873,21 @@
       <c r="BY33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BZ33" s="3" t="s">
+      <c r="BZ33" s="4" t="s">
         <v>20</v>
       </c>
       <c r="CA33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="CB33" s="4" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="CB33" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="CC33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="CD33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="CE33" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="CD33" s="3"/>
+      <c r="CE33" s="3"/>
       <c r="CF33" s="3"/>
-      <c r="CG33" s="3"/>
       <c r="CI33" s="3"/>
       <c r="CJ33" s="3"/>
       <c r="CO33" s="5">
@@ -5998,7 +5972,7 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
-      <c r="AF34" s="3"/>
+      <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
@@ -6023,7 +5997,7 @@
       <c r="BB34" s="1"/>
       <c r="BC34" s="1"/>
       <c r="BD34" s="1"/>
-      <c r="BE34" s="1"/>
+      <c r="BE34" s="3"/>
       <c r="BF34" s="3"/>
       <c r="BG34" s="3"/>
       <c r="BH34" s="3"/>
@@ -6037,10 +6011,14 @@
       <c r="BP34" s="3"/>
       <c r="BQ34" s="3"/>
       <c r="BR34" s="3"/>
-      <c r="BS34" s="3"/>
-      <c r="BT34" s="3"/>
+      <c r="BS34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT34" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="BU34" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="BV34" s="3" t="s">
         <v>20</v>
@@ -6054,28 +6032,23 @@
       <c r="BY34" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BZ34" s="3" t="s">
+      <c r="BZ34" s="4" t="s">
         <v>20</v>
       </c>
       <c r="CA34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="CB34" s="4" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="CB34" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="CC34" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="CD34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="CE34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="CF34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="CG34" s="3"/>
+      <c r="CE34" s="3"/>
+      <c r="CF34" s="3"/>
       <c r="CI34" s="3"/>
       <c r="CJ34" s="3"/>
       <c r="CO34" s="5">
@@ -6160,7 +6133,7 @@
       <c r="AC35" s="10"/>
       <c r="AD35" s="10"/>
       <c r="AE35" s="10"/>
-      <c r="AF35" s="10"/>
+      <c r="AF35" s="9"/>
       <c r="AG35" s="9"/>
       <c r="AH35" s="9"/>
       <c r="AI35" s="9"/>
@@ -6185,7 +6158,7 @@
       <c r="BB35" s="9"/>
       <c r="BC35" s="9"/>
       <c r="BD35" s="9"/>
-      <c r="BE35" s="9"/>
+      <c r="BE35" s="10"/>
       <c r="BF35" s="10"/>
       <c r="BG35" s="10"/>
       <c r="BH35" s="10"/>
@@ -6206,23 +6179,22 @@
       <c r="BW35" s="10"/>
       <c r="BX35" s="10"/>
       <c r="BY35" s="10"/>
-      <c r="BZ35" s="10"/>
-      <c r="CA35" s="10"/>
+      <c r="CA35" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="CB35" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="CC35" s="10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CD35" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="CE35" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="CF35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="CG35" s="10" t="s">
         <v>5</v>
       </c>
+      <c r="CF35" s="10"/>
       <c r="CI35" s="10"/>
       <c r="CJ35" s="10"/>
       <c r="CO35" s="11">
@@ -6355,23 +6327,22 @@
       <c r="BY36" s="7"/>
       <c r="BZ36" s="7"/>
       <c r="CA36" s="7"/>
-      <c r="CB36" s="7"/>
+      <c r="CB36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="CC36" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="CD36" s="7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CE36" s="7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="CF36" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="CG36" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="CH36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="CI36" s="7"/>
+      <c r="CG36" s="7"/>
       <c r="CO36" s="8">
         <v>1</v>
       </c>
@@ -6503,20 +6474,19 @@
       <c r="BZ37" s="3"/>
       <c r="CA37" s="3"/>
       <c r="CB37" s="3"/>
-      <c r="CD37" s="3"/>
+      <c r="CC37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="CD37" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="CE37" s="3" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="CF37" s="3" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="CG37" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="CH37" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="CI37" s="3" t="s">
         <v>55</v>
       </c>
       <c r="CO37" s="5">
@@ -6570,25 +6540,25 @@
     <row r="39" spans="1:137" x14ac:dyDescent="0.2">
       <c r="CO39" s="4">
         <f>SUM(CO1:CO35)</f>
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:137" x14ac:dyDescent="0.2">
       <c r="CP43" s="4">
         <f>SUM(CO1:CO8)+32*SUM(CO9:CO35)+SUM(CO36:CO37)+32*SUM(Odd!DA9:DA39)+63</f>
-        <v>5229</v>
+        <v>5133</v>
       </c>
       <c r="CQ43" s="4">
-        <f>8+32*(35-9+1-1)+32*(39-9+1-1)+2</f>
-        <v>1802</v>
+        <f>8+32*(35-9+1)+32*(39-9+1)+64+1</f>
+        <v>1929</v>
       </c>
       <c r="CR43" s="12">
         <f>CP43/CQ43</f>
-        <v>2.9017758046614874</v>
+        <v>2.6609642301710732</v>
       </c>
       <c r="CS43" s="4">
         <f>1/CR43</f>
-        <v>0.34461656148403136</v>
+        <v>0.37580362361192282</v>
       </c>
     </row>
     <row r="44" spans="1:137" x14ac:dyDescent="0.2">
@@ -6614,8 +6584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ES43"/>
   <sheetViews>
-    <sheetView topLeftCell="BQ27" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20:AD20"/>
+    <sheetView topLeftCell="L15" workbookViewId="0">
+      <selection activeCell="BI31" sqref="BI31:CV39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -11094,12 +11064,14 @@
         <v>24</v>
       </c>
       <c r="BF27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BG27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BG27" s="1" t="s">
+      <c r="BH27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="BH27" s="1"/>
       <c r="BI27" s="1"/>
       <c r="BJ27" s="1"/>
       <c r="BK27" s="1"/>
@@ -11144,7 +11116,7 @@
       <c r="CY27" s="3"/>
       <c r="CZ27" s="3"/>
       <c r="DA27" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="DB27" s="3"/>
       <c r="DC27" s="3"/>
@@ -11309,8 +11281,8 @@
       <c r="BE28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="BF28" s="1" t="s">
-        <v>54</v>
+      <c r="BF28" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="BG28" s="1" t="s">
         <v>54</v>
@@ -11319,12 +11291,14 @@
         <v>54</v>
       </c>
       <c r="BI28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BJ28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BJ28" s="1" t="s">
+      <c r="BK28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="BK28" s="1"/>
       <c r="BL28" s="1"/>
       <c r="BM28" s="1"/>
       <c r="BN28" s="1"/>
@@ -11496,8 +11470,8 @@
       <c r="BH29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="BI29" s="1" t="s">
-        <v>54</v>
+      <c r="BI29" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="BJ29" s="1" t="s">
         <v>54</v>
@@ -11506,12 +11480,14 @@
         <v>54</v>
       </c>
       <c r="BL29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BM29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BM29" s="1" t="s">
+      <c r="BN29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="BN29" s="1"/>
       <c r="BO29" s="1"/>
       <c r="BP29" s="1"/>
       <c r="BQ29" s="1"/>
@@ -11679,12 +11655,14 @@
         <v>20</v>
       </c>
       <c r="BM30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BN30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BN30" s="1" t="s">
+      <c r="BO30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="BO30" s="1"/>
       <c r="BP30" s="1"/>
       <c r="BQ30" s="1"/>
       <c r="BR30" s="1"/>
@@ -11839,24 +11817,21 @@
         <v>2</v>
       </c>
       <c r="BK31" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="BL31" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="BM31" s="1" t="s">
         <v>54</v>
       </c>
       <c r="BN31" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="BO31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BP31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BQ31" s="1" t="s">
+      <c r="BP31" s="4" t="s">
         <v>5</v>
       </c>
       <c r="BR31" s="1"/>
@@ -11894,7 +11869,7 @@
       <c r="CY31" s="3"/>
       <c r="CZ31" s="3"/>
       <c r="DA31" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="DB31" s="3"/>
       <c r="DC31" s="3"/>
@@ -12017,11 +11992,11 @@
       <c r="BM32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="BN32" s="1" t="s">
+      <c r="BN32" s="4" t="s">
         <v>20</v>
       </c>
       <c r="BO32" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="BP32" s="1" t="s">
         <v>53</v>
@@ -12080,13 +12055,10 @@
       <c r="CH32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="CI32" s="1" t="s">
-        <v>53</v>
+      <c r="CI32" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="CJ32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="CK32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="CL32" s="3"/>
@@ -12288,12 +12260,9 @@
         <v>20</v>
       </c>
       <c r="CJ33" s="3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="CK33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="CL33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="CM33" s="3"/>
@@ -12651,7 +12620,7 @@
         <v>20</v>
       </c>
       <c r="CI35" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="CJ35" s="3" t="s">
         <v>24</v>
@@ -12675,12 +12644,9 @@
         <v>24</v>
       </c>
       <c r="CQ35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="CR35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="CS35" s="4" t="s">
+      <c r="CR35" s="4" t="s">
         <v>5</v>
       </c>
       <c r="CT35" s="3"/>
@@ -12860,13 +12826,13 @@
         <v>20</v>
       </c>
       <c r="CI36" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="CJ36" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CK36" s="3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="CL36" s="3" t="s">
         <v>20</v>
@@ -12887,16 +12853,13 @@
         <v>20</v>
       </c>
       <c r="CR36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="CS36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="CT36" s="4" t="s">
+      <c r="CS36" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="CT36" s="3"/>
       <c r="CU36" s="3"/>
-      <c r="CV36" s="3"/>
       <c r="CY36" s="3"/>
       <c r="CZ36" s="3"/>
       <c r="DA36" s="5">
@@ -13036,12 +12999,14 @@
       <c r="CF37" s="3"/>
       <c r="CG37" s="3"/>
       <c r="CH37" s="3"/>
-      <c r="CI37" s="3"/>
+      <c r="CI37" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="CJ37" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CK37" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="CL37" s="3" t="s">
         <v>20</v>
@@ -13058,23 +13023,20 @@
       <c r="CP37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="CQ37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="CR37" s="4" t="s">
-        <v>20</v>
+      <c r="CQ37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="CR37" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="CS37" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="CT37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="CU37" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="CU37" s="3"/>
       <c r="CV37" s="3"/>
-      <c r="CW37" s="3"/>
       <c r="CY37" s="3"/>
       <c r="CZ37" s="3"/>
       <c r="DA37" s="5">
@@ -13215,9 +13177,11 @@
       <c r="CG38" s="3"/>
       <c r="CH38" s="3"/>
       <c r="CI38" s="3"/>
-      <c r="CJ38" s="3"/>
+      <c r="CJ38" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="CK38" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="CL38" s="3" t="s">
         <v>20</v>
@@ -13234,25 +13198,22 @@
       <c r="CP38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="CQ38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="CR38" s="4" t="s">
-        <v>20</v>
+      <c r="CQ38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="CR38" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="CS38" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CT38" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="CU38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="CV38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="CW38" s="3"/>
+      <c r="CV38" s="3"/>
       <c r="CY38" s="3"/>
       <c r="CZ38" s="3"/>
       <c r="DA38" s="5">
@@ -13400,20 +13361,19 @@
       <c r="CN39" s="10"/>
       <c r="CO39" s="10"/>
       <c r="CP39" s="10"/>
-      <c r="CQ39" s="10"/>
+      <c r="CR39" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="CS39" s="10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CT39" s="10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CU39" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="CV39" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="CW39" s="10" t="s">
         <v>5</v>
       </c>
       <c r="CY39" s="10"/>
@@ -13800,7 +13760,7 @@
     <row r="43" spans="1:149" x14ac:dyDescent="0.2">
       <c r="DA43" s="4">
         <f>SUM(DA9:DA39)</f>
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>